<commit_message>
Mobile client v 0.1
</commit_message>
<xml_diff>
--- a/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
+++ b/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
@@ -20,7 +20,7 @@
     <sheet name="web.Model{C}" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Columns{C}'!$A$1:$C$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tables{T}'!$A$1:$P$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'web.Model{C}'!$A$1:$C$380</definedName>
   </definedNames>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="269">
   <si>
     <t>Schema</t>
   </si>
@@ -947,6 +947,15 @@
   </si>
   <si>
     <t>Term</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>employees</t>
+  </si>
+  <si>
+    <t>Role,Employees</t>
   </si>
 </sst>
 </file>
@@ -1384,10 +1393,10 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE26" sqref="AE26"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1678,7 @@
         <v>7</v>
       </c>
       <c r="N5" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="O5" t="s">
         <v>73</v>
@@ -2487,7 +2496,7 @@
         <v>17</v>
       </c>
       <c r="AC25" s="12" t="str">
-        <f t="shared" ref="AC25:AC26" si="5">O25</f>
+        <f t="shared" ref="AC25" si="5">O25</f>
         <v>Mitarbeiter</v>
       </c>
       <c r="AE25" t="s">
@@ -2537,13 +2546,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S104"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B105" sqref="B105"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,9 +2878,6 @@
       <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
       <c r="H10" s="7" t="s">
         <v>13</v>
       </c>
@@ -2887,10 +2893,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -2905,10 +2911,13 @@
         <v>7</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
+        <v>251</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J11" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2916,10 +2925,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -2934,10 +2943,10 @@
         <v>7</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>27</v>
+        <v>78</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2948,7 +2957,7 @@
         <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -2963,10 +2972,10 @@
         <v>7</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2977,7 +2986,7 @@
         <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -2992,10 +3001,10 @@
         <v>7</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -3006,7 +3015,7 @@
         <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -3017,11 +3026,14 @@
       <c r="F15" t="s">
         <v>7</v>
       </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
       <c r="H15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3032,7 +3044,7 @@
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -3044,10 +3056,10 @@
         <v>7</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3058,7 +3070,7 @@
         <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -3069,14 +3081,11 @@
       <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
       <c r="H17" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3084,10 +3093,10 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -3102,10 +3111,10 @@
         <v>7</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3116,7 +3125,7 @@
         <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -3131,10 +3140,10 @@
         <v>7</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3145,7 +3154,7 @@
         <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -3160,10 +3169,10 @@
         <v>7</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3171,10 +3180,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -3189,10 +3198,10 @@
         <v>7</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3203,7 +3212,7 @@
         <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -3218,10 +3227,10 @@
         <v>7</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3232,7 +3241,7 @@
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -3247,10 +3256,10 @@
         <v>7</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="I23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3261,7 +3270,7 @@
         <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -3276,10 +3285,10 @@
         <v>7</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3287,10 +3296,10 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -3305,16 +3314,10 @@
         <v>7</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="O25" s="14">
-        <v>1</v>
-      </c>
-      <c r="P25" s="14">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3325,7 +3328,7 @@
         <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -3340,13 +3343,13 @@
         <v>7</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="O26" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P26" s="14">
         <v>1</v>
@@ -3360,7 +3363,7 @@
         <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -3375,16 +3378,16 @@
         <v>7</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="O27" s="14">
         <v>2</v>
       </c>
       <c r="P27" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3395,7 +3398,7 @@
         <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -3410,13 +3413,13 @@
         <v>7</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O28" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P28" s="14">
         <v>2</v>
@@ -3430,7 +3433,7 @@
         <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -3445,16 +3448,16 @@
         <v>7</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="O29" s="14">
+        <v>1</v>
+      </c>
+      <c r="P29" s="14">
         <v>2</v>
-      </c>
-      <c r="P29" s="14">
-        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3465,7 +3468,7 @@
         <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -3476,17 +3479,20 @@
       <c r="F30" t="s">
         <v>7</v>
       </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
       <c r="H30" s="7" t="s">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O30" s="14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P30" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3497,25 +3503,28 @@
         <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
       <c r="F31" t="s">
         <v>7</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O31" s="14">
         <v>6</v>
       </c>
       <c r="P31" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3526,28 +3535,25 @@
         <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
       <c r="F32" t="s">
         <v>7</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="O32" s="14">
         <v>6</v>
       </c>
       <c r="P32" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -3558,22 +3564,25 @@
         <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
       <c r="F33" t="s">
         <v>7</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="O33" s="14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P33" s="14">
         <v>3</v>
@@ -3587,7 +3596,7 @@
         <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -3596,16 +3605,16 @@
         <v>7</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O34" s="14">
+        <v>1</v>
+      </c>
+      <c r="P34" s="14">
         <v>3</v>
-      </c>
-      <c r="P34" s="14">
-        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3616,7 +3625,7 @@
         <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -3625,16 +3634,16 @@
         <v>7</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O35" s="14">
         <v>3</v>
       </c>
       <c r="P35" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -3645,7 +3654,7 @@
         <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -3654,16 +3663,16 @@
         <v>7</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O36" s="14">
         <v>3</v>
       </c>
       <c r="P36" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -3674,7 +3683,7 @@
         <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -3683,16 +3692,16 @@
         <v>7</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O37" s="14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P37" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -3703,7 +3712,7 @@
         <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -3712,16 +3721,16 @@
         <v>7</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O38" s="14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P38" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3732,7 +3741,7 @@
         <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -3741,16 +3750,16 @@
         <v>7</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O39" s="14">
         <v>5</v>
       </c>
       <c r="P39" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3761,7 +3770,7 @@
         <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -3770,13 +3779,13 @@
         <v>7</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>201</v>
+        <v>120</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="O40" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P40" s="14">
         <v>1</v>
@@ -3790,7 +3799,7 @@
         <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -3799,16 +3808,16 @@
         <v>7</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="O41" s="14">
         <v>4</v>
       </c>
       <c r="P41" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -3819,7 +3828,7 @@
         <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -3828,16 +3837,16 @@
         <v>7</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="O42" s="14">
         <v>4</v>
       </c>
       <c r="P42" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -3848,7 +3857,7 @@
         <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -3857,13 +3866,13 @@
         <v>7</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="O43" s="14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P43" s="14">
         <v>3</v>
@@ -3877,31 +3886,28 @@
         <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
       </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
       <c r="F44" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="O44" s="14">
         <v>7</v>
       </c>
       <c r="P44" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -3909,25 +3915,28 @@
         <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
       <c r="F45" t="s">
         <v>7</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O45" s="14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P45" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3938,48 +3947,48 @@
         <v>106</v>
       </c>
       <c r="C46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="O46" s="14">
+        <v>5</v>
+      </c>
+      <c r="P46" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s">
         <v>204</v>
       </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="7" t="s">
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I47" s="7" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3990,7 +3999,7 @@
         <v>139</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -4001,11 +4010,14 @@
       <c r="F48" t="s">
         <v>7</v>
       </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
       <c r="H48" s="7" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -4016,22 +4028,22 @@
         <v>139</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
-      <c r="G49" t="s">
-        <v>7</v>
-      </c>
       <c r="H49" s="7" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -4042,22 +4054,22 @@
         <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
-      <c r="E50" t="s">
-        <v>7</v>
-      </c>
       <c r="F50" t="s">
         <v>7</v>
       </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
       <c r="H50" s="7" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -4068,7 +4080,7 @@
         <v>139</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -4080,10 +4092,10 @@
         <v>7</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -4094,7 +4106,7 @@
         <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -4106,10 +4118,10 @@
         <v>7</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -4120,7 +4132,7 @@
         <v>139</v>
       </c>
       <c r="C53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -4132,10 +4144,10 @@
         <v>7</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -4143,10 +4155,10 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>214</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -4157,14 +4169,11 @@
       <c r="F54" t="s">
         <v>7</v>
       </c>
-      <c r="G54" t="s">
-        <v>7</v>
-      </c>
       <c r="H54" s="7" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -4175,7 +4184,7 @@
         <v>214</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -4186,11 +4195,14 @@
       <c r="F55" t="s">
         <v>7</v>
       </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
       <c r="H55" s="7" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -4201,13 +4213,22 @@
         <v>214</v>
       </c>
       <c r="C56" t="s">
-        <v>211</v>
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>212</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -4215,37 +4236,16 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O57" s="14">
-        <v>1</v>
-      </c>
-      <c r="P57" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q57">
-        <v>557</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -4256,7 +4256,7 @@
         <v>225</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -4271,13 +4271,13 @@
         <v>7</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="O58" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P58" s="14">
         <v>1</v>
@@ -4294,7 +4294,7 @@
         <v>225</v>
       </c>
       <c r="C59" t="s">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -4309,22 +4309,19 @@
         <v>7</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>235</v>
+        <v>125</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="J59" t="s">
-        <v>237</v>
+        <v>109</v>
       </c>
       <c r="O59" s="14">
         <v>2</v>
       </c>
       <c r="P59" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q59">
-        <v>370</v>
+        <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -4335,25 +4332,37 @@
         <v>225</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
+      <c r="E60" t="s">
+        <v>7</v>
+      </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
       <c r="H60" s="7" t="s">
-        <v>137</v>
+        <v>235</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>122</v>
+        <v>236</v>
+      </c>
+      <c r="J60" t="s">
+        <v>237</v>
       </c>
       <c r="O60" s="14">
         <v>2</v>
       </c>
       <c r="P60" s="14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="Q60">
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -4364,7 +4373,7 @@
         <v>225</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -4372,20 +4381,17 @@
       <c r="F61" t="s">
         <v>7</v>
       </c>
-      <c r="G61" t="s">
-        <v>7</v>
-      </c>
       <c r="H61" s="7" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="O61" s="14">
+        <v>2</v>
+      </c>
+      <c r="P61" s="14">
         <v>3</v>
-      </c>
-      <c r="P61" s="14">
-        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -4396,14 +4402,11 @@
         <v>225</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
-      <c r="E62" t="s">
-        <v>7</v>
-      </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
@@ -4411,10 +4414,10 @@
         <v>7</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="O62" s="14">
         <v>3</v>
@@ -4431,11 +4434,14 @@
         <v>225</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
       <c r="F63" t="s">
         <v>7</v>
       </c>
@@ -4443,10 +4449,10 @@
         <v>7</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O63" s="14">
         <v>3</v>
@@ -4463,32 +4469,29 @@
         <v>225</v>
       </c>
       <c r="C64" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
-      <c r="E64" t="s">
-        <v>7</v>
-      </c>
       <c r="F64" t="s">
         <v>7</v>
       </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
       <c r="H64" s="7" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="O64" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P64" s="14">
         <v>1</v>
       </c>
-      <c r="Q64">
-        <v>557</v>
-      </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -4498,28 +4501,31 @@
         <v>225</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
+      <c r="E65" t="s">
+        <v>7</v>
+      </c>
       <c r="F65" t="s">
         <v>7</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="O65" s="14">
         <v>4</v>
       </c>
       <c r="P65" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q65">
-        <v>370</v>
+        <v>557</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -4530,28 +4536,28 @@
         <v>225</v>
       </c>
       <c r="C66" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
       </c>
-      <c r="E66" t="s">
-        <v>7</v>
-      </c>
       <c r="F66" t="s">
         <v>7</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O66" s="14">
         <v>4</v>
       </c>
       <c r="P66" s="14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="Q66">
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -4562,7 +4568,7 @@
         <v>225</v>
       </c>
       <c r="C67" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -4574,16 +4580,16 @@
         <v>7</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="O67" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P67" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -4594,7 +4600,7 @@
         <v>225</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -4606,10 +4612,10 @@
         <v>7</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O68" s="14">
         <v>5</v>
@@ -4626,7 +4632,7 @@
         <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -4638,10 +4644,10 @@
         <v>7</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O69" s="14">
         <v>5</v>
@@ -4655,10 +4661,10 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -4669,24 +4675,18 @@
       <c r="F70" t="s">
         <v>7</v>
       </c>
-      <c r="G70" t="s">
-        <v>7</v>
-      </c>
       <c r="H70" s="7" t="s">
-        <v>228</v>
+        <v>164</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="O70" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P70" s="14">
         <v>1</v>
       </c>
-      <c r="Q70">
-        <v>557</v>
-      </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -4696,7 +4696,7 @@
         <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -4711,13 +4711,13 @@
         <v>7</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>125</v>
+        <v>228</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="O71" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P71" s="14">
         <v>1</v>
@@ -4734,7 +4734,7 @@
         <v>217</v>
       </c>
       <c r="C72" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -4745,23 +4745,23 @@
       <c r="F72" t="s">
         <v>7</v>
       </c>
+      <c r="G72" t="s">
+        <v>7</v>
+      </c>
       <c r="H72" s="7" t="s">
-        <v>215</v>
+        <v>125</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="J72" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="O72" s="14">
         <v>2</v>
       </c>
       <c r="P72" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q72">
-        <v>370</v>
+        <v>557</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -4772,7 +4772,7 @@
         <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -4783,23 +4783,20 @@
       <c r="F73" t="s">
         <v>7</v>
       </c>
-      <c r="G73" t="s">
-        <v>7</v>
-      </c>
       <c r="H73" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="J73" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="O73" s="14">
         <v>2</v>
       </c>
       <c r="P73" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q73">
         <v>370</v>
@@ -4813,11 +4810,14 @@
         <v>217</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
       </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
       <c r="F74" t="s">
         <v>7</v>
       </c>
@@ -4825,16 +4825,22 @@
         <v>7</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>169</v>
+        <v>236</v>
+      </c>
+      <c r="J74" t="s">
+        <v>239</v>
       </c>
       <c r="O74" s="14">
+        <v>2</v>
+      </c>
+      <c r="P74" s="14">
         <v>3</v>
       </c>
-      <c r="P74" s="14">
-        <v>1</v>
+      <c r="Q74">
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -4845,14 +4851,11 @@
         <v>217</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
       </c>
-      <c r="E75" t="s">
-        <v>7</v>
-      </c>
       <c r="F75" t="s">
         <v>7</v>
       </c>
@@ -4860,10 +4863,10 @@
         <v>7</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="O75" s="14">
         <v>3</v>
@@ -4880,11 +4883,14 @@
         <v>217</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
       </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
       <c r="F76" t="s">
         <v>7</v>
       </c>
@@ -4892,10 +4898,10 @@
         <v>7</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O76" s="14">
         <v>3</v>
@@ -4912,7 +4918,7 @@
         <v>217</v>
       </c>
       <c r="C77" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -4920,21 +4926,21 @@
       <c r="F77" t="s">
         <v>7</v>
       </c>
+      <c r="G77" t="s">
+        <v>7</v>
+      </c>
       <c r="H77" s="7" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="O77" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P77" s="14">
         <v>1</v>
       </c>
-      <c r="Q77">
-        <v>557</v>
-      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -4944,7 +4950,7 @@
         <v>217</v>
       </c>
       <c r="C78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -4953,19 +4959,19 @@
         <v>7</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="O78" s="14">
         <v>4</v>
       </c>
       <c r="P78" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q78">
-        <v>370</v>
+        <v>557</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -4976,7 +4982,7 @@
         <v>217</v>
       </c>
       <c r="C79" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -4985,16 +4991,19 @@
         <v>7</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="I79" s="7" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="O79" s="14">
         <v>4</v>
       </c>
       <c r="P79" s="14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="Q79">
+        <v>370</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -5005,7 +5014,7 @@
         <v>217</v>
       </c>
       <c r="C80" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -5014,16 +5023,16 @@
         <v>7</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="O80" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P80" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -5034,7 +5043,7 @@
         <v>217</v>
       </c>
       <c r="C81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -5043,10 +5052,10 @@
         <v>7</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O81" s="14">
         <v>5</v>
@@ -5063,7 +5072,7 @@
         <v>217</v>
       </c>
       <c r="C82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -5072,10 +5081,10 @@
         <v>7</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O82" s="14">
         <v>5</v>
@@ -5089,10 +5098,10 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C83" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -5100,14 +5109,17 @@
       <c r="F83" t="s">
         <v>7</v>
       </c>
-      <c r="G83" t="s">
-        <v>7</v>
-      </c>
       <c r="H83" s="7" t="s">
-        <v>218</v>
+        <v>164</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>219</v>
+        <v>157</v>
+      </c>
+      <c r="O83" s="14">
+        <v>5</v>
+      </c>
+      <c r="P83" s="14">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -5118,14 +5130,11 @@
         <v>226</v>
       </c>
       <c r="C84" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
       </c>
-      <c r="E84" t="s">
-        <v>7</v>
-      </c>
       <c r="F84" t="s">
         <v>7</v>
       </c>
@@ -5133,13 +5142,10 @@
         <v>7</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="J84" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -5150,7 +5156,7 @@
         <v>226</v>
       </c>
       <c r="C85" t="s">
-        <v>152</v>
+        <v>227</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -5165,10 +5171,13 @@
         <v>7</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>153</v>
+        <v>229</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>152</v>
+        <v>229</v>
+      </c>
+      <c r="J85" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -5176,10 +5185,10 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="D86" t="s">
         <v>7</v>
@@ -5194,10 +5203,10 @@
         <v>7</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="I86" s="7" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -5208,7 +5217,7 @@
         <v>246</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
@@ -5219,11 +5228,14 @@
       <c r="F87" t="s">
         <v>7</v>
       </c>
+      <c r="G87" t="s">
+        <v>7</v>
+      </c>
       <c r="H87" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I87" t="s">
-        <v>122</v>
+        <v>27</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -5231,10 +5243,10 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D88" t="s">
         <v>7</v>
@@ -5245,14 +5257,11 @@
       <c r="F88" t="s">
         <v>7</v>
       </c>
-      <c r="G88" t="s">
-        <v>7</v>
-      </c>
       <c r="H88" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="I88" s="7" t="s">
-        <v>255</v>
+        <v>137</v>
+      </c>
+      <c r="I88" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -5263,7 +5272,7 @@
         <v>248</v>
       </c>
       <c r="C89" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D89" t="s">
         <v>7</v>
@@ -5274,11 +5283,14 @@
       <c r="F89" t="s">
         <v>7</v>
       </c>
+      <c r="G89" t="s">
+        <v>7</v>
+      </c>
       <c r="H89" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I89" t="s">
-        <v>122</v>
+        <v>254</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -5289,7 +5301,7 @@
         <v>248</v>
       </c>
       <c r="C90" t="s">
-        <v>253</v>
+        <v>122</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
@@ -5301,10 +5313,10 @@
         <v>7</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="I90" s="7" t="s">
-        <v>257</v>
+        <v>137</v>
+      </c>
+      <c r="I90" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -5312,10 +5324,10 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>253</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
@@ -5326,20 +5338,11 @@
       <c r="F91" t="s">
         <v>7</v>
       </c>
-      <c r="G91" t="s">
-        <v>7</v>
-      </c>
       <c r="H91" s="7" t="s">
-        <v>125</v>
+        <v>256</v>
       </c>
       <c r="I91" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="O91" s="14">
-        <v>2</v>
-      </c>
-      <c r="P91" s="14">
-        <v>1</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -5350,7 +5353,7 @@
         <v>249</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
@@ -5365,13 +5368,13 @@
         <v>7</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="I92" s="7" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="O92" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P92" s="14">
         <v>1</v>
@@ -5385,7 +5388,7 @@
         <v>249</v>
       </c>
       <c r="C93" t="s">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
@@ -5396,17 +5399,20 @@
       <c r="F93" t="s">
         <v>7</v>
       </c>
+      <c r="G93" t="s">
+        <v>7</v>
+      </c>
       <c r="H93" s="7" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
       <c r="O93" s="14">
         <v>1</v>
       </c>
       <c r="P93" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -5417,7 +5423,7 @@
         <v>249</v>
       </c>
       <c r="C94" t="s">
-        <v>258</v>
+        <v>147</v>
       </c>
       <c r="D94" t="s">
         <v>7</v>
@@ -5428,20 +5434,14 @@
       <c r="F94" t="s">
         <v>7</v>
       </c>
-      <c r="G94" t="s">
-        <v>7</v>
-      </c>
       <c r="H94" s="7" t="s">
-        <v>250</v>
+        <v>148</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="J94" t="s">
-        <v>262</v>
+        <v>149</v>
       </c>
       <c r="O94" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P94" s="14">
         <v>2</v>
@@ -5455,7 +5455,7 @@
         <v>249</v>
       </c>
       <c r="C95" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D95" t="s">
         <v>7</v>
@@ -5470,19 +5470,19 @@
         <v>7</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>88</v>
+        <v>250</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>88</v>
+        <v>247</v>
       </c>
       <c r="J95" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="O95" s="14">
         <v>2</v>
       </c>
       <c r="P95" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -5493,25 +5493,34 @@
         <v>249</v>
       </c>
       <c r="C96" t="s">
-        <v>110</v>
+        <v>259</v>
       </c>
       <c r="D96" t="s">
         <v>7</v>
       </c>
+      <c r="E96" t="s">
+        <v>7</v>
+      </c>
       <c r="F96" t="s">
         <v>7</v>
       </c>
+      <c r="G96" t="s">
+        <v>7</v>
+      </c>
       <c r="H96" s="7" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+      <c r="J96" t="s">
+        <v>260</v>
       </c>
       <c r="O96" s="14">
+        <v>2</v>
+      </c>
+      <c r="P96" s="14">
         <v>3</v>
-      </c>
-      <c r="P96" s="14">
-        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -5522,7 +5531,7 @@
         <v>249</v>
       </c>
       <c r="C97" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D97" t="s">
         <v>7</v>
@@ -5531,16 +5540,16 @@
         <v>7</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O97" s="14">
         <v>3</v>
       </c>
       <c r="P97" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -5551,7 +5560,7 @@
         <v>249</v>
       </c>
       <c r="C98" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
@@ -5560,16 +5569,16 @@
         <v>7</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I98" s="7" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="O98" s="14">
         <v>3</v>
       </c>
       <c r="P98" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
@@ -5580,7 +5589,7 @@
         <v>249</v>
       </c>
       <c r="C99" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D99" t="s">
         <v>7</v>
@@ -5589,16 +5598,16 @@
         <v>7</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I99" t="s">
-        <v>122</v>
+        <v>128</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="O99" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P99" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -5609,7 +5618,7 @@
         <v>249</v>
       </c>
       <c r="C100" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -5618,16 +5627,16 @@
         <v>7</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I100" s="7" t="s">
-        <v>115</v>
+        <v>137</v>
+      </c>
+      <c r="I100" t="s">
+        <v>122</v>
       </c>
       <c r="O100" s="14">
         <v>4</v>
       </c>
       <c r="P100" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -5638,7 +5647,7 @@
         <v>249</v>
       </c>
       <c r="C101" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D101" t="s">
         <v>7</v>
@@ -5647,16 +5656,16 @@
         <v>7</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O101" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P101" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
@@ -5667,7 +5676,7 @@
         <v>249</v>
       </c>
       <c r="C102" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D102" t="s">
         <v>7</v>
@@ -5676,16 +5685,16 @@
         <v>7</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O102" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P102" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -5696,7 +5705,7 @@
         <v>249</v>
       </c>
       <c r="C103" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D103" t="s">
         <v>7</v>
@@ -5705,16 +5714,16 @@
         <v>7</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O103" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P103" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -5725,7 +5734,7 @@
         <v>249</v>
       </c>
       <c r="C104" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D104" t="s">
         <v>7</v>
@@ -5734,20 +5743,49 @@
         <v>7</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O104" s="14">
         <v>5</v>
       </c>
       <c r="P104" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="O105" s="14">
+        <v>5</v>
+      </c>
+      <c r="P105" s="14">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C10"/>
+  <autoFilter ref="A1:C11"/>
   <sortState ref="A2:N586">
     <sortCondition ref="B2:B586"/>
   </sortState>

</xml_diff>

<commit_message>
employees color and scheduler
</commit_message>
<xml_diff>
--- a/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
+++ b/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="299">
   <si>
     <t>Schema</t>
   </si>
@@ -1043,6 +1043,9 @@
   </si>
   <si>
     <t>Werkzeug</t>
+  </si>
+  <si>
+    <t>IsColorElement</t>
   </si>
 </sst>
 </file>
@@ -1479,11 +1482,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="N11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="V8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomRight" activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,6 +2597,9 @@
       <c r="X25" t="s">
         <v>7</v>
       </c>
+      <c r="Y25" t="s">
+        <v>7</v>
+      </c>
       <c r="AB25" s="14">
         <v>17</v>
       </c>
@@ -2840,13 +2846,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S107"/>
+  <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H56" sqref="H56"/>
+      <selection pane="bottomRight" activeCell="T102" sqref="T102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2871,7 @@
     <col min="15" max="16" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2923,8 +2929,11 @@
       <c r="S1" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2953,7 +2962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2979,7 +2988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3037,7 +3046,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3069,7 +3078,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3098,7 +3107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3153,7 +3162,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -3214,7 +3223,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3243,7 +3252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3272,7 +3281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3301,7 +3310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3330,7 +3339,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -5808,7 +5817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -5837,7 +5846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -5866,7 +5875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -5895,7 +5904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -5924,7 +5933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -5953,22 +5962,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="C102" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="D102" t="s">
         <v>7</v>
       </c>
-      <c r="E102" t="s">
-        <v>7</v>
-      </c>
       <c r="F102" t="s">
         <v>7</v>
       </c>
@@ -5976,13 +5982,22 @@
         <v>7</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>270</v>
+        <v>164</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="O102" s="14">
+        <v>1</v>
+      </c>
+      <c r="P102" s="14">
+        <v>3</v>
+      </c>
+      <c r="T102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -5990,7 +6005,7 @@
         <v>268</v>
       </c>
       <c r="C103" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="D103" t="s">
         <v>7</v>
@@ -6005,13 +6020,13 @@
         <v>7</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>125</v>
+        <v>270</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -6019,7 +6034,7 @@
         <v>268</v>
       </c>
       <c r="C104" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D104" t="s">
         <v>7</v>
@@ -6030,14 +6045,17 @@
       <c r="F104" t="s">
         <v>7</v>
       </c>
+      <c r="G104" t="s">
+        <v>7</v>
+      </c>
       <c r="H104" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -6045,7 +6063,7 @@
         <v>268</v>
       </c>
       <c r="C105" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="D105" t="s">
         <v>7</v>
@@ -6056,17 +6074,14 @@
       <c r="F105" t="s">
         <v>7</v>
       </c>
-      <c r="G105" t="s">
-        <v>7</v>
-      </c>
       <c r="H105" s="7" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -6074,7 +6089,7 @@
         <v>268</v>
       </c>
       <c r="C106" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="D106" t="s">
         <v>7</v>
@@ -6089,13 +6104,13 @@
         <v>7</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -6103,21 +6118,50 @@
         <v>268</v>
       </c>
       <c r="C107" t="s">
+        <v>86</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" t="s">
+        <v>7</v>
+      </c>
+      <c r="F107" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" t="s">
+        <v>268</v>
+      </c>
+      <c r="C108" t="s">
         <v>272</v>
       </c>
-      <c r="D107" t="s">
-        <v>7</v>
-      </c>
-      <c r="E107" t="s">
-        <v>7</v>
-      </c>
-      <c r="F107" t="s">
-        <v>7</v>
-      </c>
-      <c r="H107" s="7" t="s">
+      <c r="D108" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" t="s">
+        <v>7</v>
+      </c>
+      <c r="H108" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="I107" s="7" t="s">
+      <c r="I108" s="7" t="s">
         <v>274</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Instruments - show employee name
</commit_message>
<xml_diff>
--- a/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
+++ b/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="306">
   <si>
     <t>Schema</t>
   </si>
@@ -1503,11 +1503,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="U11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P36" sqref="P36"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,6 +2707,12 @@
       <c r="X27" t="s">
         <v>7</v>
       </c>
+      <c r="Y27" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>7</v>
+      </c>
       <c r="AC27" s="14">
         <v>18</v>
       </c>
@@ -2940,7 +2946,7 @@
   <dimension ref="A1:T108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C85" sqref="C85"/>
@@ -6294,13 +6300,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,6 +6368,17 @@
         <v>225</v>
       </c>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Profit reports employee salary
</commit_message>
<xml_diff>
--- a/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
+++ b/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="339">
   <si>
     <t>Schema</t>
   </si>
@@ -907,9 +907,6 @@
     <t>autos</t>
   </si>
   <si>
-    <t>Autos,JobPositions</t>
-  </si>
-  <si>
     <t>jobPositions</t>
   </si>
   <si>
@@ -1093,15 +1090,6 @@
     <t>employeeRates</t>
   </si>
   <si>
-    <t>CustomPrice</t>
-  </si>
-  <si>
-    <t>Spezial</t>
-  </si>
-  <si>
-    <t>Special</t>
-  </si>
-  <si>
     <t>employeeId</t>
   </si>
   <si>
@@ -1154,6 +1142,30 @@
   </si>
   <si>
     <t>Invoice payment</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Einkommen</t>
+  </si>
+  <si>
+    <t>SalaryType</t>
+  </si>
+  <si>
+    <t>Salary type</t>
+  </si>
+  <si>
+    <t>Einkommentyp</t>
+  </si>
+  <si>
+    <t>salaryTypes</t>
+  </si>
+  <si>
+    <t>JobPositions,SalaryTypes</t>
+  </si>
+  <si>
+    <t>Autos,JobPositions,SalaryTypes</t>
   </si>
 </sst>
 </file>
@@ -1590,11 +1602,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC20" sqref="AC20"/>
+      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1719,7 @@
         <v>209</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AC1" s="13" t="s">
         <v>65</v>
@@ -1879,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="N5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O5" t="s">
         <v>73</v>
@@ -1921,7 +1933,7 @@
         <v>7</v>
       </c>
       <c r="N6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="O6" t="s">
         <v>225</v>
@@ -1960,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -1978,10 +1990,10 @@
         <v>7</v>
       </c>
       <c r="O7" t="s">
+        <v>301</v>
+      </c>
+      <c r="P7" t="s">
         <v>302</v>
-      </c>
-      <c r="P7" t="s">
-        <v>303</v>
       </c>
       <c r="R7" t="s">
         <v>7</v>
@@ -2026,7 +2038,7 @@
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="O8" t="s">
         <v>82</v>
@@ -2274,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="N14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="O14" t="s">
         <v>227</v>
@@ -2505,7 +2517,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
@@ -2523,10 +2535,10 @@
         <v>176</v>
       </c>
       <c r="O20" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="P20" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
@@ -2630,7 +2642,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C24" t="s">
         <v>44</v>
@@ -2645,10 +2657,10 @@
         <v>7</v>
       </c>
       <c r="L24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O24" t="s">
         <v>228</v>
@@ -2729,7 +2741,7 @@
         <v>7</v>
       </c>
       <c r="N26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O26" t="s">
         <v>87</v>
@@ -2741,16 +2753,16 @@
         <v>7</v>
       </c>
       <c r="S26" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="T26" t="s">
         <v>276</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="U26" s="7" t="s">
+      <c r="V26" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="V26" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="W26" t="s">
         <v>106</v>
@@ -2786,7 +2798,7 @@
         <v>7</v>
       </c>
       <c r="N27" t="s">
-        <v>252</v>
+        <v>338</v>
       </c>
       <c r="O27" t="s">
         <v>242</v>
@@ -2798,16 +2810,16 @@
         <v>7</v>
       </c>
       <c r="S27" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="T27" t="s">
         <v>312</v>
       </c>
-      <c r="T27" t="s">
-        <v>313</v>
-      </c>
       <c r="U27" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="V27" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="V27" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="W27" t="s">
         <v>27</v>
@@ -2834,7 +2846,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
@@ -2846,10 +2858,10 @@
         <v>7</v>
       </c>
       <c r="O28" t="s">
+        <v>254</v>
+      </c>
+      <c r="P28" t="s">
         <v>255</v>
-      </c>
-      <c r="P28" t="s">
-        <v>256</v>
       </c>
       <c r="R28" t="s">
         <v>7</v>
@@ -2860,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -2878,13 +2890,13 @@
         <v>7</v>
       </c>
       <c r="N29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="O29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="W29" t="s">
         <v>27</v>
@@ -2914,7 +2926,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
@@ -2926,10 +2938,10 @@
         <v>7</v>
       </c>
       <c r="O30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
@@ -2937,7 +2949,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C31" t="s">
         <v>44</v>
@@ -2949,10 +2961,10 @@
         <v>7</v>
       </c>
       <c r="O31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y31" t="s">
         <v>7</v>
@@ -2969,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
@@ -2981,10 +2993,10 @@
         <v>7</v>
       </c>
       <c r="O32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
@@ -2992,7 +3004,7 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
@@ -3004,10 +3016,10 @@
         <v>7</v>
       </c>
       <c r="O33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R33" t="s">
         <v>7</v>
@@ -3018,7 +3030,7 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -3030,10 +3042,10 @@
         <v>7</v>
       </c>
       <c r="O34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="R34" t="s">
         <v>7</v>
@@ -3044,7 +3056,7 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
@@ -3056,10 +3068,10 @@
         <v>7</v>
       </c>
       <c r="O35" t="s">
+        <v>291</v>
+      </c>
+      <c r="P35" t="s">
         <v>292</v>
-      </c>
-      <c r="P35" t="s">
-        <v>293</v>
       </c>
       <c r="R35" t="s">
         <v>7</v>
@@ -3070,7 +3082,7 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
@@ -3082,10 +3094,10 @@
         <v>7</v>
       </c>
       <c r="O36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R36" t="s">
         <v>7</v>
@@ -3096,7 +3108,7 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
@@ -3105,10 +3117,10 @@
         <v>55</v>
       </c>
       <c r="O37" t="s">
+        <v>298</v>
+      </c>
+      <c r="P37" t="s">
         <v>299</v>
-      </c>
-      <c r="P37" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.25">
@@ -3116,7 +3128,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
@@ -3137,10 +3149,10 @@
         <v>237</v>
       </c>
       <c r="O38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R38" t="s">
         <v>7</v>
@@ -3161,7 +3173,7 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -3176,19 +3188,19 @@
         <v>7</v>
       </c>
       <c r="L39" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="M39" t="s">
         <v>240</v>
       </c>
       <c r="N39" t="s">
-        <v>237</v>
+        <v>337</v>
       </c>
       <c r="O39" t="s">
+        <v>309</v>
+      </c>
+      <c r="P39" t="s">
         <v>310</v>
-      </c>
-      <c r="P39" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
@@ -3196,7 +3208,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -3214,13 +3226,13 @@
         <v>7</v>
       </c>
       <c r="N40" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="O40" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="P40" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="R40" t="s">
         <v>7</v>
@@ -3241,7 +3253,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
@@ -3253,10 +3265,10 @@
         <v>7</v>
       </c>
       <c r="O41" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="P41" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="R41" t="s">
         <v>7</v>
@@ -3267,7 +3279,7 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
@@ -3285,10 +3297,10 @@
         <v>7</v>
       </c>
       <c r="O42" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="P42" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="R42" t="s">
         <v>7</v>
@@ -3324,13 +3336,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T123"/>
+  <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,7 +3420,7 @@
         <v>229</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -3677,7 +3689,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -3698,7 +3710,7 @@
         <v>243</v>
       </c>
       <c r="J11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3787,28 +3799,28 @@
         <v>80</v>
       </c>
       <c r="C15" t="s">
+        <v>303</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="J15" t="s">
         <v>305</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="J15" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -3819,7 +3831,7 @@
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -3840,7 +3852,7 @@
         <v>89</v>
       </c>
       <c r="J16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -5116,7 +5128,7 @@
         <v>7</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>106</v>
@@ -5276,7 +5288,7 @@
         <v>221</v>
       </c>
       <c r="C65" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -5294,7 +5306,7 @@
         <v>89</v>
       </c>
       <c r="J65" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="O65" s="14">
         <v>3</v>
@@ -5506,22 +5518,22 @@
         <v>221</v>
       </c>
       <c r="C72" t="s">
+        <v>270</v>
+      </c>
+      <c r="D72" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="D72" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" s="7" t="s">
+      <c r="I72" s="7" t="s">
         <v>272</v>
-      </c>
-      <c r="I72" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="O72" s="14">
         <v>5</v>
@@ -5538,22 +5550,22 @@
         <v>221</v>
       </c>
       <c r="C73" t="s">
+        <v>263</v>
+      </c>
+      <c r="D73" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D73" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" t="s">
-        <v>7</v>
-      </c>
-      <c r="H73" s="7" t="s">
+      <c r="I73" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="I73" s="7" t="s">
-        <v>266</v>
       </c>
       <c r="O73" s="14">
         <v>5</v>
@@ -5760,7 +5772,7 @@
         <v>213</v>
       </c>
       <c r="C79" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -5778,7 +5790,7 @@
         <v>89</v>
       </c>
       <c r="J79" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="O79" s="14">
         <v>3</v>
@@ -6468,7 +6480,7 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C103" t="s">
         <v>27</v>
@@ -6486,7 +6498,7 @@
         <v>7</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I103" s="7" t="s">
         <v>27</v>
@@ -6497,7 +6509,7 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C104" t="s">
         <v>106</v>
@@ -6526,7 +6538,7 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C105" t="s">
         <v>119</v>
@@ -6552,7 +6564,7 @@
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C106" t="s">
         <v>157</v>
@@ -6581,10 +6593,10 @@
         <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C107" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
@@ -6605,7 +6617,7 @@
         <v>89</v>
       </c>
       <c r="J107" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
@@ -6613,25 +6625,25 @@
         <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C108" t="s">
+        <v>263</v>
+      </c>
+      <c r="D108" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" t="s">
+        <v>7</v>
+      </c>
+      <c r="H108" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D108" t="s">
-        <v>7</v>
-      </c>
-      <c r="E108" t="s">
-        <v>7</v>
-      </c>
-      <c r="F108" t="s">
-        <v>7</v>
-      </c>
-      <c r="H108" s="7" t="s">
+      <c r="I108" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="I108" s="7" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
@@ -6639,7 +6651,7 @@
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C109" t="s">
         <v>27</v>
@@ -6668,7 +6680,7 @@
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C110" t="s">
         <v>249</v>
@@ -6692,7 +6704,7 @@
         <v>238</v>
       </c>
       <c r="J110" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
@@ -6700,7 +6712,7 @@
         <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C111" t="s">
         <v>84</v>
@@ -6729,7 +6741,7 @@
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C112" t="s">
         <v>93</v>
@@ -6758,7 +6770,7 @@
         <v>11</v>
       </c>
       <c r="B113" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C113" t="s">
         <v>94</v>
@@ -6787,10 +6799,10 @@
         <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C114" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
@@ -6813,7 +6825,7 @@
         <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C115" t="s">
         <v>249</v>
@@ -6837,7 +6849,7 @@
         <v>238</v>
       </c>
       <c r="J115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
@@ -6845,7 +6857,7 @@
         <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C116" t="s">
         <v>93</v>
@@ -6874,7 +6886,7 @@
         <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C117" t="s">
         <v>94</v>
@@ -6903,10 +6915,10 @@
         <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C118" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D118" t="s">
         <v>7</v>
@@ -6917,11 +6929,14 @@
       <c r="F118" t="s">
         <v>7</v>
       </c>
+      <c r="G118" t="s">
+        <v>7</v>
+      </c>
       <c r="H118" s="7" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="I118" s="7" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -6929,10 +6944,10 @@
         <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C119" t="s">
-        <v>27</v>
+        <v>333</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
@@ -6947,10 +6962,13 @@
         <v>7</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>27</v>
+        <v>335</v>
       </c>
       <c r="I119" s="7" t="s">
-        <v>27</v>
+        <v>334</v>
+      </c>
+      <c r="J119" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -6958,10 +6976,10 @@
         <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C120" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -6976,10 +6994,10 @@
         <v>7</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="I120" s="7" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -6987,10 +7005,10 @@
         <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C121" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
@@ -7001,11 +7019,14 @@
       <c r="F121" t="s">
         <v>7</v>
       </c>
+      <c r="G121" t="s">
+        <v>7</v>
+      </c>
       <c r="H121" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
@@ -7013,10 +7034,10 @@
         <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C122" t="s">
-        <v>331</v>
+        <v>87</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
@@ -7027,17 +7048,11 @@
       <c r="F122" t="s">
         <v>7</v>
       </c>
-      <c r="G122" t="s">
-        <v>7</v>
-      </c>
       <c r="H122" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I122" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J122" t="s">
-        <v>330</v>
+        <v>87</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -7045,27 +7060,59 @@
         <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="C123" t="s">
+        <v>327</v>
+      </c>
+      <c r="D123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123" t="s">
+        <v>7</v>
+      </c>
+      <c r="G123" t="s">
+        <v>7</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J123" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>11</v>
+      </c>
+      <c r="B124" t="s">
+        <v>320</v>
+      </c>
+      <c r="C124" t="s">
         <v>92</v>
       </c>
-      <c r="D123" t="s">
-        <v>7</v>
-      </c>
-      <c r="E123" t="s">
-        <v>7</v>
-      </c>
-      <c r="F123" t="s">
-        <v>7</v>
-      </c>
-      <c r="G123" t="s">
-        <v>7</v>
-      </c>
-      <c r="H123" s="7" t="s">
+      <c r="D124" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F124" t="s">
+        <v>7</v>
+      </c>
+      <c r="G124" t="s">
+        <v>7</v>
+      </c>
+      <c r="H124" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I123" s="7" t="s">
+      <c r="I124" s="7" t="s">
         <v>92</v>
       </c>
     </row>
@@ -7192,7 +7239,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Missing materials for auto
</commit_message>
<xml_diff>
--- a/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
+++ b/ProfiCraftsman/ProfiCraftsman/Generation/ProfiCraftsman.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="351">
   <si>
     <t>Schema</t>
   </si>
@@ -1117,9 +1117,6 @@
     <t>Proceeds accounts</t>
   </si>
   <si>
-    <t>ProductTypes,ProductAmountTypes,ProceedsAccounts</t>
-  </si>
-  <si>
     <t>AdditionalCostTypes,ProceedsAccounts</t>
   </si>
   <si>
@@ -1199,6 +1196,12 @@
   </si>
   <si>
     <t>Summe</t>
+  </si>
+  <si>
+    <t>ProductTypes,ProductAmountTypes,ProceedsAccounts,MaterialAmountTypes</t>
+  </si>
+  <si>
+    <t>Instruments,MaterialAmountTypes</t>
   </si>
 </sst>
 </file>
@@ -1635,11 +1638,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,7 +1969,7 @@
         <v>7</v>
       </c>
       <c r="N6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O6" t="s">
         <v>224</v>
@@ -2005,7 +2008,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -2017,10 +2020,10 @@
         <v>7</v>
       </c>
       <c r="O7" t="s">
+        <v>338</v>
+      </c>
+      <c r="P7" t="s">
         <v>339</v>
-      </c>
-      <c r="P7" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -2094,10 +2097,10 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P9" t="s">
         <v>81</v>
@@ -2342,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="N15" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="O15" t="s">
         <v>226</v>
@@ -2573,7 +2576,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -2591,10 +2594,10 @@
         <v>175</v>
       </c>
       <c r="O21" t="s">
+        <v>327</v>
+      </c>
+      <c r="P21" t="s">
         <v>328</v>
-      </c>
-      <c r="P21" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
@@ -2797,7 +2800,7 @@
         <v>7</v>
       </c>
       <c r="N27" t="s">
-        <v>258</v>
+        <v>350</v>
       </c>
       <c r="O27" t="s">
         <v>86</v>
@@ -2854,7 +2857,7 @@
         <v>7</v>
       </c>
       <c r="N28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O28" t="s">
         <v>241</v>
@@ -3250,7 +3253,7 @@
         <v>239</v>
       </c>
       <c r="N40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O40" t="s">
         <v>308</v>
@@ -3380,7 +3383,7 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
@@ -3401,10 +3404,10 @@
         <v>319</v>
       </c>
       <c r="O44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P44" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R44" t="s">
         <v>7</v>
@@ -3431,7 +3434,7 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
@@ -3449,13 +3452,13 @@
         <v>7</v>
       </c>
       <c r="N45" t="s">
+        <v>345</v>
+      </c>
+      <c r="O45" t="s">
         <v>346</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>347</v>
-      </c>
-      <c r="P45" t="s">
-        <v>348</v>
       </c>
       <c r="R45" t="s">
         <v>7</v>
@@ -3490,8 +3493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
@@ -3983,7 +3986,7 @@
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -4004,7 +4007,7 @@
         <v>88</v>
       </c>
       <c r="J16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -5443,7 +5446,7 @@
         <v>220</v>
       </c>
       <c r="C65" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -5461,7 +5464,7 @@
         <v>88</v>
       </c>
       <c r="J65" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O65" s="14">
         <v>3</v>
@@ -5927,7 +5930,7 @@
         <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -5945,7 +5948,7 @@
         <v>88</v>
       </c>
       <c r="J79" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O79" s="14">
         <v>3</v>
@@ -6751,7 +6754,7 @@
         <v>258</v>
       </c>
       <c r="C107" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
@@ -6772,7 +6775,7 @@
         <v>88</v>
       </c>
       <c r="J107" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
@@ -7073,25 +7076,25 @@
         <v>307</v>
       </c>
       <c r="C118" t="s">
+        <v>329</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" t="s">
+        <v>7</v>
+      </c>
+      <c r="G118" t="s">
+        <v>7</v>
+      </c>
+      <c r="H118" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="D118" t="s">
-        <v>7</v>
-      </c>
-      <c r="E118" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" t="s">
-        <v>7</v>
-      </c>
-      <c r="G118" t="s">
-        <v>7</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>331</v>
-      </c>
       <c r="I118" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -7102,28 +7105,28 @@
         <v>307</v>
       </c>
       <c r="C119" t="s">
+        <v>331</v>
+      </c>
+      <c r="D119" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" t="s">
+        <v>7</v>
+      </c>
+      <c r="G119" t="s">
+        <v>7</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="I119" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="D119" t="s">
-        <v>7</v>
-      </c>
-      <c r="E119" t="s">
-        <v>7</v>
-      </c>
-      <c r="F119" t="s">
-        <v>7</v>
-      </c>
-      <c r="G119" t="s">
-        <v>7</v>
-      </c>
-      <c r="H119" s="7" t="s">
+      <c r="J119" t="s">
         <v>334</v>
-      </c>
-      <c r="I119" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="J119" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -7218,7 +7221,7 @@
         <v>313</v>
       </c>
       <c r="C123" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D123" t="s">
         <v>7</v>
@@ -7239,7 +7242,7 @@
         <v>88</v>
       </c>
       <c r="J123" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -7276,7 +7279,7 @@
         <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C125" t="s">
         <v>17</v>
@@ -7305,7 +7308,7 @@
         <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C126" t="s">
         <v>83</v>
@@ -7334,10 +7337,10 @@
         <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C127" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D127" t="s">
         <v>7</v>
@@ -7358,7 +7361,7 @@
         <v>88</v>
       </c>
       <c r="J127" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -7366,7 +7369,7 @@
         <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C128" t="s">
         <v>92</v>
@@ -7395,7 +7398,7 @@
         <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C129" t="s">
         <v>93</v>
@@ -7421,7 +7424,7 @@
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C130" t="s">
         <v>255</v>
@@ -7453,7 +7456,7 @@
         <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C131" t="s">
         <v>17</v>
@@ -7479,7 +7482,7 @@
         <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C132" t="s">
         <v>83</v>
@@ -7497,7 +7500,7 @@
         <v>7</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I132" s="7" t="s">
         <v>83</v>
@@ -7508,10 +7511,10 @@
         <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C133" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D133" t="s">
         <v>7</v>
@@ -7532,7 +7535,7 @@
         <v>88</v>
       </c>
       <c r="J133" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -7540,7 +7543,7 @@
         <v>11</v>
       </c>
       <c r="B134" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C134" t="s">
         <v>92</v>
@@ -7569,7 +7572,7 @@
         <v>11</v>
       </c>
       <c r="B135" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C135" t="s">
         <v>93</v>

</xml_diff>